<commit_message>
11/27; UR dashboard not updated since 11/25
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisun/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5951CBD5-BF61-244A-B04A-D5651D47EED6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B107DAC-E096-9245-B771-1D11DE0109CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{2DC10746-11EF-284B-92B6-91815D32F896}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9E3710-B2DD-D440-8104-3784AF9C3D06}">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1706,6 +1706,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>44161</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>44162</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12/7; not updated on 12/5,12/6
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisun/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1515688E-8231-124B-848C-420EBFD12FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C86866-476C-FB43-B12F-01B187813335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{2DC10746-11EF-284B-92B6-91815D32F896}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9E3710-B2DD-D440-8104-3784AF9C3D06}">
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1805,6 +1805,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>44170</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>44171</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>44172</v>
+      </c>
+      <c r="B130">
+        <v>47</v>
+      </c>
+      <c r="C130">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12/10; adjusted plotly scale factors
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisun/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9973F-FC41-7A46-9136-E7357DE0D00B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C418F85-51AA-A14A-8F50-675BE5EAD101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{2DC10746-11EF-284B-92B6-91815D32F896}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9E3710-B2DD-D440-8104-3784AF9C3D06}">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1860,6 +1860,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>44175</v>
+      </c>
+      <c r="B133">
+        <v>35</v>
+      </c>
+      <c r="C133">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12/11; adjusted plotly widths
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisun/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C418F85-51AA-A14A-8F50-675BE5EAD101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B4EBD7-A955-884F-BE3A-0934D142460B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{2DC10746-11EF-284B-92B6-91815D32F896}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9E3710-B2DD-D440-8104-3784AF9C3D06}">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+      <selection activeCell="G133" sqref="G133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1871,6 +1871,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>44176</v>
+      </c>
+      <c r="B134">
+        <v>39</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12/24; fixed time bloc graphs
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -390,7 +390,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D145" sqref="D145"/>
+      <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2015,7 +2015,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1">
+        <v>44189</v>
+      </c>
+      <c r="B147">
+        <v>36</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
1/17; separated data processing to dataproc.r
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -2,37 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF66E3C7-27C1-0747-8848-763E88CD1C11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D6DE44-6309-F34C-984B-B8BA685B0F3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="covdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -52,10 +35,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,19 +44,315 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Verdana"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -84,19 +360,208 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,19 +870,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2286,13 +2748,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>44213</v>
+      </c>
+      <c r="B171">
+        <v>23</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2/1; truncate daily positivity rates
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093D2B5-AE2C-C34F-970B-4BA35557D699}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B48A6F-8FD9-2F4E-9FCB-6B395ED850B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="D186" sqref="D186"/>
+      <selection activeCell="G181" sqref="G181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2913,6 +2913,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B186">
+        <v>349</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
2/3; "New positives" are 3, but this isn't reflected in the graphic
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3244E1-891D-BC44-9E5E-32DE16689B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E18155-F0B5-8E46-8E12-1898D4D25BF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="F190" sqref="F190"/>
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2935,6 +2935,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>44230</v>
+      </c>
+      <c r="B188">
+        <v>89</v>
+      </c>
+      <c r="C188">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
2/6; First day post "dangerous up-tick" email
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB0AF8-9F2E-354C-AEA4-0A928EA5DFB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEEEA37-C792-CE4C-88BD-4B438D15A936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1640" windowWidth="25600" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covdata" sheetId="1" r:id="rId1"/>
@@ -870,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="E190" sqref="E190"/>
+      <selection activeCell="A190" sqref="A190:A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2968,6 +2968,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>44233</v>
+      </c>
+      <c r="B191">
+        <v>76</v>
+      </c>
+      <c r="C191">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
2/15; added note about offical dashboard update
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F729B7E7-A552-414F-BE97-C94961A630C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E936C0-A8B3-424F-AEF9-2BA234FB1A9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="H199" sqref="H199"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="D200" sqref="D200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3067,6 +3067,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>44242</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
2/23; Official UR dashboard combined Students,Staff,Faculty by campus location
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14187B4B-8224-0142-B0E2-DC6BC0A1AA19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE0C3D-E298-FD47-9E69-704D276ADBA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="B213" sqref="B213"/>
+      <selection activeCell="C210" sqref="C210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3155,6 +3155,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>44250</v>
+      </c>
+      <c r="B208">
+        <v>360</v>
+      </c>
+      <c r="C208">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
3/6; graphics on UR's dashboard did not update to include 3/6 data. "Tests" was extrapolated from "Total Test Results since August 1st" html text box
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9F7020-B146-E047-8083-2FCBC7EE2D3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486BCEF4-9CA3-B540-842B-9EFE8849457A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="G221" sqref="G221"/>
+      <selection activeCell="F219" sqref="F219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3287,6 +3287,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>44261</v>
+      </c>
+      <c r="B219">
+        <v>370</v>
+      </c>
+      <c r="C219">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
3/7; graphic on official dashboard updated to include 3/6 data (1 day late)
</commit_message>
<xml_diff>
--- a/covdata.xlsx
+++ b/covdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisunorig/Desktop/UR Covid Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486BCEF4-9CA3-B540-842B-9EFE8849457A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB28FF61-9AB3-794F-9896-AE2B67E57D3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -881,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="F219" sqref="F219"/>
+      <selection activeCell="G219" sqref="G219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3298,6 +3298,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>44262</v>
+      </c>
+      <c r="B220">
+        <v>19</v>
+      </c>
+      <c r="C220">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>